<commit_message>
Cannith bracers have ins phys and magical sheltering
</commit_message>
<xml_diff>
--- a/data-builder/cannith-crafting.xlsx
+++ b/data-builder/cannith-crafting.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzinman\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8520" firstSheet="28" activeTab="38"/>
   </bookViews>
@@ -55,7 +50,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="38" hidden="1">Sheet1!$A$1:$CF$212</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2981" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="263">
   <si>
     <t>Min Level</t>
   </si>
@@ -852,11 +847,14 @@
   <si>
     <t>Sort</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1220,7 +1218,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1233,7 +1231,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2924,7 +2922,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4254,7 +4252,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4488,7 +4486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4734,7 +4732,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5150,7 +5148,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5420,7 +5418,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8071,7 +8069,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8710,7 +8708,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8974,7 +8972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9226,7 +9224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10365,7 +10363,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10635,7 +10633,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10875,7 +10873,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11383,7 +11381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11775,7 +11773,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -13069,7 +13067,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15669,7 +15667,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15911,7 +15909,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -17657,7 +17655,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -18037,7 +18035,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -18283,7 +18281,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -18559,7 +18557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -20073,7 +20071,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -21337,7 +21335,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -21577,7 +21575,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -22650,9 +22648,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -22849,7 +22847,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -22962,7 +22960,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>210</v>
       </c>
@@ -23081,7 +23079,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -23200,7 +23198,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>247</v>
       </c>
@@ -23313,7 +23311,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>248</v>
       </c>
@@ -23426,7 +23424,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>249</v>
       </c>
@@ -23539,7 +23537,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>250</v>
       </c>
@@ -23652,7 +23650,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>251</v>
       </c>
@@ -23765,7 +23763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>229</v>
       </c>
@@ -23902,7 +23900,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>259</v>
       </c>
@@ -24015,7 +24013,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>252</v>
       </c>
@@ -24125,7 +24123,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>128</v>
       </c>
@@ -24244,7 +24242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>254</v>
       </c>
@@ -24357,7 +24355,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>253</v>
       </c>
@@ -24467,7 +24465,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>255</v>
       </c>
@@ -24580,7 +24578,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>228</v>
       </c>
@@ -24702,7 +24700,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>245</v>
       </c>
@@ -24815,7 +24813,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>227</v>
       </c>
@@ -24949,7 +24947,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>260</v>
       </c>
@@ -25062,7 +25060,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>246</v>
       </c>
@@ -25187,7 +25185,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>256</v>
       </c>
@@ -25306,7 +25304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -25419,7 +25417,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -25532,7 +25530,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:65" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>218</v>
       </c>
@@ -25651,7 +25649,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -25764,7 +25762,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>258</v>
       </c>
@@ -25889,7 +25887,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26248,7 +26246,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26702,7 +26700,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -27867,7 +27865,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -28761,7 +28759,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -28958,60 +28956,60 @@
   <dimension ref="A1:CF212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BJ206" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CC5" sqref="CC5"/>
+      <selection pane="bottomRight" activeCell="Z72" sqref="Z72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="35" width="3.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="35" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.42578125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="75" max="76" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="5.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="75" max="76" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="5.77734375" style="1"/>
+    <col min="82" max="82" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="5.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:84" s="5" customFormat="1" ht="20.45" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -29265,7 +29263,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>110</v>
       </c>
@@ -29430,7 +29428,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>114</v>
       </c>
@@ -29599,7 +29597,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>231</v>
       </c>
@@ -29764,7 +29762,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>232</v>
       </c>
@@ -29929,7 +29927,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="6" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>233</v>
       </c>
@@ -30094,7 +30092,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>230</v>
       </c>
@@ -30259,7 +30257,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>123</v>
       </c>
@@ -30424,7 +30422,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>125</v>
       </c>
@@ -30591,7 +30589,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="10" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>111</v>
       </c>
@@ -30758,7 +30756,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>113</v>
       </c>
@@ -30925,7 +30923,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>115</v>
       </c>
@@ -31092,7 +31090,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="13" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>117</v>
       </c>
@@ -31257,7 +31255,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>120</v>
       </c>
@@ -31424,7 +31422,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>121</v>
       </c>
@@ -31593,7 +31591,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>124</v>
       </c>
@@ -31760,7 +31758,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>126</v>
       </c>
@@ -31927,7 +31925,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="18" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -32100,7 +32098,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>197</v>
       </c>
@@ -32265,7 +32263,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>196</v>
       </c>
@@ -32430,7 +32428,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>198</v>
       </c>
@@ -32595,7 +32593,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>109</v>
       </c>
@@ -32758,7 +32756,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="23" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>116</v>
       </c>
@@ -32925,7 +32923,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>4</v>
       </c>
@@ -33088,7 +33086,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>210</v>
       </c>
@@ -33255,7 +33253,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="26" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -33378,7 +33376,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>247</v>
       </c>
@@ -33541,7 +33539,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="28" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>248</v>
       </c>
@@ -33704,7 +33702,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="29" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>249</v>
       </c>
@@ -33867,7 +33865,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>250</v>
       </c>
@@ -34030,7 +34028,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>251</v>
       </c>
@@ -34193,7 +34191,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>229</v>
       </c>
@@ -34372,7 +34370,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="33" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>259</v>
       </c>
@@ -34535,7 +34533,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="34" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>252</v>
       </c>
@@ -34696,7 +34694,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="35" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>128</v>
       </c>
@@ -34863,7 +34861,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="36" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>254</v>
       </c>
@@ -35026,7 +35024,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="37" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>253</v>
       </c>
@@ -35187,7 +35185,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="38" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>255</v>
       </c>
@@ -35350,7 +35348,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="39" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>228</v>
       </c>
@@ -35519,7 +35517,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="40" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>245</v>
       </c>
@@ -35682,7 +35680,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="41" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>227</v>
       </c>
@@ -35859,7 +35857,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="42" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>260</v>
       </c>
@@ -36022,7 +36020,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="43" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>246</v>
       </c>
@@ -36193,7 +36191,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="44" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>256</v>
       </c>
@@ -36360,7 +36358,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="45" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>226</v>
       </c>
@@ -36523,7 +36521,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="46" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>257</v>
       </c>
@@ -36686,7 +36684,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="47" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>218</v>
       </c>
@@ -36853,7 +36851,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="48" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>26</v>
       </c>
@@ -37016,7 +37014,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="49" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>258</v>
       </c>
@@ -37179,7 +37177,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="50" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>219</v>
       </c>
@@ -37344,7 +37342,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="51" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>220</v>
       </c>
@@ -37509,7 +37507,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="52" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>221</v>
       </c>
@@ -37674,7 +37672,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="53" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>222</v>
       </c>
@@ -37839,7 +37837,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="54" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>223</v>
       </c>
@@ -38004,7 +38002,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="55" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>224</v>
       </c>
@@ -38169,7 +38167,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="56" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>225</v>
       </c>
@@ -38334,7 +38332,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="57" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>199</v>
       </c>
@@ -38501,7 +38499,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="58" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>21</v>
       </c>
@@ -38664,7 +38662,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="59" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
@@ -38835,7 +38833,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="60" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>211</v>
       </c>
@@ -39004,7 +39002,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="61" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>212</v>
       </c>
@@ -39173,7 +39171,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="62" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>213</v>
       </c>
@@ -39342,7 +39340,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="63" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>214</v>
       </c>
@@ -39511,7 +39509,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="64" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>215</v>
       </c>
@@ -39680,7 +39678,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="65" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>216</v>
       </c>
@@ -39849,7 +39847,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="66" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>217</v>
       </c>
@@ -40018,7 +40016,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="67" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>182</v>
       </c>
@@ -40187,7 +40185,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="68" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -40362,7 +40360,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="69" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>9</v>
       </c>
@@ -40527,7 +40525,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="70" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>164</v>
       </c>
@@ -40640,7 +40638,9 @@
       <c r="AN70" s="3"/>
       <c r="AO70" s="3"/>
       <c r="AP70" s="3"/>
-      <c r="AQ70" s="3"/>
+      <c r="AQ70" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="AR70" s="3"/>
       <c r="AS70" s="3"/>
       <c r="AT70" s="3"/>
@@ -40696,7 +40696,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="71" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>163</v>
       </c>
@@ -40809,7 +40809,9 @@
       <c r="AN71" s="3"/>
       <c r="AO71" s="3"/>
       <c r="AP71" s="3"/>
-      <c r="AQ71" s="3"/>
+      <c r="AQ71" s="3" t="s">
+        <v>262</v>
+      </c>
       <c r="AR71" s="3"/>
       <c r="AS71" s="3"/>
       <c r="AT71" s="3"/>
@@ -40865,7 +40867,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="72" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -41036,7 +41038,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="73" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>6</v>
       </c>
@@ -41205,7 +41207,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="74" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>148</v>
       </c>
@@ -41374,7 +41376,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="75" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>151</v>
       </c>
@@ -41543,7 +41545,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="76" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>153</v>
       </c>
@@ -41712,7 +41714,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="77" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
@@ -41879,7 +41881,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="78" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>149</v>
       </c>
@@ -42048,7 +42050,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="79" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>17</v>
       </c>
@@ -42215,7 +42217,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="80" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>152</v>
       </c>
@@ -42382,7 +42384,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="81" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>18</v>
       </c>
@@ -42549,7 +42551,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="82" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>23</v>
       </c>
@@ -42718,7 +42720,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="83" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>25</v>
       </c>
@@ -42887,7 +42889,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="84" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>154</v>
       </c>
@@ -43054,7 +43056,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="85" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>244</v>
       </c>
@@ -43217,7 +43219,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="86" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -43396,7 +43398,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="87" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -43561,7 +43563,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="88" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -43728,7 +43730,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="89" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
@@ -43893,7 +43895,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="90" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -44060,7 +44062,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="91" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
@@ -44225,7 +44227,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="92" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
@@ -44392,7 +44394,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="93" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -44557,7 +44559,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="94" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
@@ -44732,7 +44734,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="95" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
@@ -44897,7 +44899,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="96" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -45062,7 +45064,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="97" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
@@ -45235,7 +45237,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="98" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
@@ -45400,7 +45402,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="99" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
@@ -45567,7 +45569,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="100" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -45736,7 +45738,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="101" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
@@ -45905,7 +45907,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="102" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -46074,7 +46076,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="103" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
@@ -46243,7 +46245,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="104" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
@@ -46410,7 +46412,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="105" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
@@ -46581,7 +46583,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="106" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>62</v>
       </c>
@@ -46750,7 +46752,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="107" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>59</v>
       </c>
@@ -46923,7 +46925,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="108" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>58</v>
       </c>
@@ -47092,7 +47094,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="109" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>8</v>
       </c>
@@ -47263,7 +47265,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="110" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>60</v>
       </c>
@@ -47432,7 +47434,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="111" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>14</v>
       </c>
@@ -47601,7 +47603,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="112" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>19</v>
       </c>
@@ -47770,7 +47772,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="113" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>57</v>
       </c>
@@ -47941,7 +47943,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="114" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>61</v>
       </c>
@@ -48110,7 +48112,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="115" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>181</v>
       </c>
@@ -48281,7 +48283,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="116" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>180</v>
       </c>
@@ -48452,7 +48454,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="117" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>106</v>
       </c>
@@ -48621,7 +48623,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="118" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>105</v>
       </c>
@@ -48792,7 +48794,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="119" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
@@ -48961,7 +48963,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="120" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
@@ -49124,7 +49126,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="121" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>157</v>
       </c>
@@ -49295,7 +49297,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="122" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>156</v>
       </c>
@@ -49466,7 +49468,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="123" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>158</v>
       </c>
@@ -49637,7 +49639,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="124" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>155</v>
       </c>
@@ -49808,7 +49810,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="125" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>160</v>
       </c>
@@ -49979,7 +49981,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="126" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>161</v>
       </c>
@@ -50150,7 +50152,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="127" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>162</v>
       </c>
@@ -50321,7 +50323,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="128" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>159</v>
       </c>
@@ -50492,7 +50494,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="129" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>10</v>
       </c>
@@ -50659,7 +50661,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="130" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>122</v>
       </c>
@@ -50830,7 +50832,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="131" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>1</v>
       </c>
@@ -50995,7 +50997,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="132" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>2</v>
       </c>
@@ -51162,7 +51164,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="133" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>7</v>
       </c>
@@ -51333,7 +51335,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="134" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>20</v>
       </c>
@@ -51500,7 +51502,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="135" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>64</v>
       </c>
@@ -51673,7 +51675,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="136" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>65</v>
       </c>
@@ -51844,7 +51846,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="137" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>66</v>
       </c>
@@ -52011,7 +52013,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="138" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>67</v>
       </c>
@@ -52184,7 +52186,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="139" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>68</v>
       </c>
@@ -52351,7 +52353,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="140" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>69</v>
       </c>
@@ -52516,7 +52518,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="141" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>70</v>
       </c>
@@ -52685,7 +52687,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="142" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>71</v>
       </c>
@@ -52852,7 +52854,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="143" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>72</v>
       </c>
@@ -53031,7 +53033,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="144" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>73</v>
       </c>
@@ -53196,7 +53198,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="145" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>74</v>
       </c>
@@ -53361,7 +53363,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="146" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>75</v>
       </c>
@@ -53538,7 +53540,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="147" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>76</v>
       </c>
@@ -53707,7 +53709,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="148" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>77</v>
       </c>
@@ -53874,7 +53876,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="149" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>78</v>
       </c>
@@ -54043,7 +54045,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="150" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>79</v>
       </c>
@@ -54212,7 +54214,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="151" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>80</v>
       </c>
@@ -54385,7 +54387,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="152" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>81</v>
       </c>
@@ -54552,7 +54554,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="153" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>82</v>
       </c>
@@ -54719,7 +54721,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="154" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>83</v>
       </c>
@@ -54894,7 +54896,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="155" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>22</v>
       </c>
@@ -55067,7 +55069,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="156" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>166</v>
       </c>
@@ -55244,7 +55246,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="157" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>165</v>
       </c>
@@ -55421,7 +55423,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="158" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>24</v>
       </c>
@@ -55586,7 +55588,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="159" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>27</v>
       </c>
@@ -55747,7 +55749,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="160" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>168</v>
       </c>
@@ -55922,7 +55924,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="161" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>167</v>
       </c>
@@ -56097,7 +56099,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="162" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>169</v>
       </c>
@@ -56272,7 +56274,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="163" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>11</v>
       </c>
@@ -56447,7 +56449,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="164" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>174</v>
       </c>
@@ -56622,7 +56624,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="165" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>171</v>
       </c>
@@ -56797,7 +56799,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="166" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>172</v>
       </c>
@@ -56972,7 +56974,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="167" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>173</v>
       </c>
@@ -57147,7 +57149,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="168" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>170</v>
       </c>
@@ -57320,7 +57322,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="169" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>193</v>
       </c>
@@ -57485,7 +57487,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="170" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>194</v>
       </c>
@@ -57650,7 +57652,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="171" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>195</v>
       </c>
@@ -57815,7 +57817,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="172" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>234</v>
       </c>
@@ -57986,7 +57988,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="173" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>235</v>
       </c>
@@ -58157,7 +58159,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="174" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>238</v>
       </c>
@@ -58328,7 +58330,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="175" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>236</v>
       </c>
@@ -58499,7 +58501,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="176" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>239</v>
       </c>
@@ -58670,7 +58672,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="177" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>237</v>
       </c>
@@ -58841,7 +58843,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="178" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>240</v>
       </c>
@@ -59012,7 +59014,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="179" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>241</v>
       </c>
@@ -59183,7 +59185,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="180" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>242</v>
       </c>
@@ -59354,7 +59356,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="181" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>243</v>
       </c>
@@ -59525,7 +59527,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="182" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>13</v>
       </c>
@@ -59692,7 +59694,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="183" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>127</v>
       </c>
@@ -59853,7 +59855,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="184" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>175</v>
       </c>
@@ -60028,7 +60030,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="185" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>176</v>
       </c>
@@ -60203,7 +60205,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="186" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>177</v>
       </c>
@@ -60378,7 +60380,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="187" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>178</v>
       </c>
@@ -60553,7 +60555,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="188" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>179</v>
       </c>
@@ -60728,7 +60730,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="189" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>16</v>
       </c>
@@ -60891,7 +60893,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="190" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>200</v>
       </c>
@@ -61062,7 +61064,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="191" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>201</v>
       </c>
@@ -61233,7 +61235,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="192" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>202</v>
       </c>
@@ -61402,7 +61404,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="193" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>118</v>
       </c>
@@ -61569,7 +61571,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="194" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>203</v>
       </c>
@@ -61740,7 +61742,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="195" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>204</v>
       </c>
@@ -61911,7 +61913,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="196" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>205</v>
       </c>
@@ -62082,7 +62084,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="197" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>206</v>
       </c>
@@ -62253,7 +62255,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="198" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>207</v>
       </c>
@@ -62424,7 +62426,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="199" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>208</v>
       </c>
@@ -62595,7 +62597,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="200" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>209</v>
       </c>
@@ -62766,7 +62768,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="201" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>28</v>
       </c>
@@ -62939,7 +62941,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="202" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>183</v>
       </c>
@@ -63120,7 +63122,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="203" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>184</v>
       </c>
@@ -63301,7 +63303,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="204" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>185</v>
       </c>
@@ -63482,7 +63484,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="205" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>12</v>
       </c>
@@ -63653,7 +63655,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="206" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>186</v>
       </c>
@@ -63834,7 +63836,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="207" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>187</v>
       </c>
@@ -64015,7 +64017,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="208" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>188</v>
       </c>
@@ -64196,7 +64198,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="209" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>189</v>
       </c>
@@ -64377,7 +64379,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="210" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>190</v>
       </c>
@@ -64558,7 +64560,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="211" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>191</v>
       </c>
@@ -64739,7 +64741,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="212" spans="1:84" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>192</v>
       </c>
@@ -64954,7 +64956,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -65194,7 +65196,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -65994,7 +65996,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -66228,7 +66230,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -66480,7 +66482,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -67869,7 +67871,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Bug fixes from feedback
</commit_message>
<xml_diff>
--- a/data-builder/cannith-crafting.xlsx
+++ b/data-builder/cannith-crafting.xlsx
@@ -48,7 +48,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="38" hidden="1">Sheet1!$A$1:$CF$212</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="38" hidden="1">Sheet1!$A$1:$CF$211</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="265">
   <si>
     <t>Min Level</t>
   </si>
@@ -850,6 +850,12 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>Sheltering</t>
+  </si>
+  <si>
+    <t>True Seeing</t>
+  </si>
 </sst>
 </file>
 
@@ -1218,7 +1224,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -28953,19 +28959,20 @@
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:CF212"/>
+  <dimension ref="A1:CF211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z72" sqref="Z72"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="2.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" style="1" customWidth="1"/>
     <col min="10" max="35" width="3.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -36360,7 +36367,7 @@
     </row>
     <row r="45" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
@@ -41714,7 +41721,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="77" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>150</v>
       </c>
@@ -41881,7 +41888,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="78" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>149</v>
       </c>
@@ -42050,7 +42057,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="79" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>17</v>
       </c>
@@ -42217,7 +42224,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="80" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>152</v>
       </c>
@@ -42384,7 +42391,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="81" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>18</v>
       </c>
@@ -42551,7 +42558,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="82" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>23</v>
       </c>
@@ -42720,7 +42727,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="83" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>25</v>
       </c>
@@ -42889,7 +42896,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="84" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>154</v>
       </c>
@@ -43056,7 +43063,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="85" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>244</v>
       </c>
@@ -43219,7 +43226,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="86" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>84</v>
       </c>
@@ -43398,7 +43405,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="87" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>85</v>
       </c>
@@ -43563,7 +43570,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="88" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>86</v>
       </c>
@@ -43730,7 +43737,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="89" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>87</v>
       </c>
@@ -43895,7 +43902,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="90" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>88</v>
       </c>
@@ -44062,7 +44069,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="91" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>89</v>
       </c>
@@ -44227,7 +44234,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="92" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>90</v>
       </c>
@@ -44394,7 +44401,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="93" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -44559,7 +44566,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="94" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>92</v>
       </c>
@@ -44734,7 +44741,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="95" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>93</v>
       </c>
@@ -44899,7 +44906,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="96" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>94</v>
       </c>
@@ -45064,7 +45071,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="97" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>95</v>
       </c>
@@ -45237,7 +45244,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="98" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>96</v>
       </c>
@@ -45402,7 +45409,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="99" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>97</v>
       </c>
@@ -45569,7 +45576,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="100" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>98</v>
       </c>
@@ -45738,7 +45745,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="101" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>99</v>
       </c>
@@ -45907,7 +45914,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="102" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>100</v>
       </c>
@@ -46076,7 +46083,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="103" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>101</v>
       </c>
@@ -46245,7 +46252,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="104" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>102</v>
       </c>
@@ -46412,7 +46419,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="105" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>103</v>
       </c>
@@ -46583,7 +46590,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="106" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>62</v>
       </c>
@@ -46752,7 +46759,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="107" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>59</v>
       </c>
@@ -46925,7 +46932,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="108" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>58</v>
       </c>
@@ -47094,7 +47101,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="109" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>8</v>
       </c>
@@ -47265,7 +47272,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="110" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>60</v>
       </c>
@@ -47434,7 +47441,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="111" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>14</v>
       </c>
@@ -47603,7 +47610,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="112" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>19</v>
       </c>
@@ -47772,7 +47779,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="113" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>57</v>
       </c>
@@ -47943,7 +47950,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="114" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>61</v>
       </c>
@@ -48112,7 +48119,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="115" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>181</v>
       </c>
@@ -48283,7 +48290,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="116" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>180</v>
       </c>
@@ -48454,7 +48461,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="117" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>106</v>
       </c>
@@ -48623,7 +48630,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="118" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>105</v>
       </c>
@@ -48794,7 +48801,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="119" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
@@ -48963,7 +48970,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="120" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
@@ -49126,7 +49133,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="121" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>157</v>
       </c>
@@ -49297,7 +49304,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="122" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>156</v>
       </c>
@@ -49468,7 +49475,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="123" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>158</v>
       </c>
@@ -49639,7 +49646,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="124" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>155</v>
       </c>
@@ -49810,7 +49817,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="125" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>160</v>
       </c>
@@ -49981,7 +49988,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="126" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>161</v>
       </c>
@@ -50152,7 +50159,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="127" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>162</v>
       </c>
@@ -50323,7 +50330,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="128" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>159</v>
       </c>
@@ -50494,7 +50501,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="129" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>10</v>
       </c>
@@ -50661,7 +50668,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="130" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>122</v>
       </c>
@@ -50828,11 +50835,11 @@
         <v>63</v>
       </c>
       <c r="CF130" s="1" t="str">
-        <f t="shared" ref="CF130:CF193" si="2">IF(AND(B130=B129,C130=C129,D130=D129,E130=E129,F130=F129,G130=G129,H130=H129,I130=I129,J130=J129,K130=K129,L130=L129,M130=M129,N130=N129,O130=O129,P130=P129,Q130=Q129,R130=R129,S130=S129,T130=T129,U130=U129,V130=V129,W130=W129,X130=X129,Y130=Y129,Z130=Z129,AA130=AA129,AB130=AB129,AC130=AC129,AD130=AD129,AE130=AE129,AF130=AF129,AG130=AG129,AH130=AH129,AI130=AI129),"YES","NO")</f>
+        <f t="shared" ref="CF130:CF192" si="2">IF(AND(B130=B129,C130=C129,D130=D129,E130=E129,F130=F129,G130=G129,H130=H129,I130=I129,J130=J129,K130=K129,L130=L129,M130=M129,N130=N129,O130=O129,P130=P129,Q130=Q129,R130=R129,S130=S129,T130=T129,U130=U129,V130=V129,W130=W129,X130=X129,Y130=Y129,Z130=Z129,AA130=AA129,AB130=AB129,AC130=AC129,AD130=AD129,AE130=AE129,AF130=AF129,AG130=AG129,AH130=AH129,AI130=AI129),"YES","NO")</f>
         <v>NO</v>
       </c>
     </row>
-    <row r="131" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>1</v>
       </c>
@@ -50997,7 +51004,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="132" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>2</v>
       </c>
@@ -51164,7 +51171,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="133" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>7</v>
       </c>
@@ -51335,7 +51342,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="134" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>20</v>
       </c>
@@ -51502,7 +51509,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="135" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>64</v>
       </c>
@@ -51675,7 +51682,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="136" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>65</v>
       </c>
@@ -51846,7 +51853,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="137" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>66</v>
       </c>
@@ -52013,7 +52020,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="138" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>67</v>
       </c>
@@ -52186,7 +52193,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="139" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>68</v>
       </c>
@@ -52353,7 +52360,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="140" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>69</v>
       </c>
@@ -52518,7 +52525,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="141" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>70</v>
       </c>
@@ -52687,7 +52694,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="142" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>71</v>
       </c>
@@ -52854,7 +52861,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="143" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>72</v>
       </c>
@@ -53033,7 +53040,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="144" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>73</v>
       </c>
@@ -53198,7 +53205,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="145" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>74</v>
       </c>
@@ -53363,7 +53370,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="146" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>75</v>
       </c>
@@ -53540,7 +53547,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="147" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>76</v>
       </c>
@@ -53709,7 +53716,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="148" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>77</v>
       </c>
@@ -53876,7 +53883,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="149" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>78</v>
       </c>
@@ -54045,7 +54052,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="150" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>79</v>
       </c>
@@ -54214,7 +54221,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="151" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>80</v>
       </c>
@@ -54387,7 +54394,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="152" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>81</v>
       </c>
@@ -54554,7 +54561,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="153" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>82</v>
       </c>
@@ -54721,7 +54728,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="154" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>83</v>
       </c>
@@ -54896,7 +54903,7 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="155" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>22</v>
       </c>
@@ -55069,9 +55076,9 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="156" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>166</v>
+        <v>263</v>
       </c>
       <c r="B156" s="3">
         <v>3</v>
@@ -55241,14 +55248,14 @@
         <v>63</v>
       </c>
       <c r="CE156" s="3"/>
-      <c r="CF156" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
+      <c r="CF156" s="1" t="e">
+        <f>IF(AND(B156=#REF!,C156=#REF!,D156=#REF!,E156=#REF!,F156=#REF!,G156=#REF!,H156=#REF!,I156=#REF!,J156=#REF!,K156=#REF!,L156=#REF!,M156=#REF!,N156=#REF!,O156=#REF!,P156=#REF!,Q156=#REF!,R156=#REF!,S156=#REF!,T156=#REF!,U156=#REF!,V156=#REF!,W156=#REF!,X156=#REF!,Y156=#REF!,Z156=#REF!,AA156=#REF!,AB156=#REF!,AC156=#REF!,AD156=#REF!,AE156=#REF!,AF156=#REF!,AG156=#REF!,AH156=#REF!,AI156=#REF!),"YES","NO")</f>
+        <v>#REF!</v>
       </c>
     </row>
-    <row r="157" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>165</v>
+        <v>24</v>
       </c>
       <c r="B157" s="3">
         <v>3</v>
@@ -55278,93 +55285,91 @@
         <v>13</v>
       </c>
       <c r="K157" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L157" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M157" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N157" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O157" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="P157" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q157" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="R157" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="S157" s="3">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="T157" s="3">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="U157" s="3">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="V157" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="W157" s="3">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="X157" s="3">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Y157" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Z157" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AA157" s="3">
         <v>30</v>
       </c>
       <c r="AB157" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AC157" s="3">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AD157" s="3">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AE157" s="3">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="AF157" s="3">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="AG157" s="3">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="AH157" s="3">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="AI157" s="3">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="AJ157" s="3"/>
       <c r="AK157" s="3"/>
       <c r="AL157" s="3"/>
-      <c r="AM157" s="3"/>
-      <c r="AN157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AM157" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN157" s="3"/>
       <c r="AO157" s="3"/>
       <c r="AP157" s="3"/>
       <c r="AQ157" s="3"/>
-      <c r="AR157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AR157" s="3"/>
       <c r="AS157" s="3"/>
       <c r="AT157" s="3"/>
       <c r="AU157" s="3"/>
@@ -55374,27 +55379,21 @@
       <c r="AY157" s="3"/>
       <c r="AZ157" s="3"/>
       <c r="BA157" s="3"/>
-      <c r="BB157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BB157" s="3"/>
       <c r="BC157" s="3"/>
       <c r="BD157" s="3"/>
       <c r="BE157" s="3"/>
-      <c r="BF157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF157" s="3"/>
       <c r="BG157" s="3"/>
-      <c r="BH157" s="3"/>
-      <c r="BI157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BH157" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BI157" s="3"/>
       <c r="BJ157" s="3"/>
       <c r="BK157" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BL157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BL157" s="3"/>
       <c r="BM157" s="3"/>
       <c r="BN157" s="3"/>
       <c r="BO157" s="3"/>
@@ -55406,135 +55405,129 @@
       <c r="BU157" s="3"/>
       <c r="BV157" s="3"/>
       <c r="BW157" s="3"/>
-      <c r="BX157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BX157" s="3"/>
       <c r="BY157" s="3"/>
       <c r="BZ157" s="3"/>
       <c r="CA157" s="3"/>
       <c r="CB157" s="3"/>
       <c r="CC157" s="3"/>
-      <c r="CD157" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CD157" s="3"/>
       <c r="CE157" s="3"/>
       <c r="CF157" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="158" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B158" s="3">
+        <v>4</v>
+      </c>
+      <c r="C158" s="3">
+        <v>6</v>
+      </c>
+      <c r="D158" s="3">
+        <v>7</v>
+      </c>
+      <c r="E158" s="3">
+        <v>10</v>
+      </c>
+      <c r="F158" s="3">
+        <v>12</v>
+      </c>
+      <c r="G158" s="3">
+        <v>13</v>
+      </c>
+      <c r="H158" s="3">
+        <v>15</v>
+      </c>
+      <c r="I158" s="3">
+        <v>16</v>
+      </c>
+      <c r="J158" s="3">
+        <v>17</v>
+      </c>
+      <c r="K158" s="3">
+        <v>19</v>
+      </c>
+      <c r="L158" s="3">
+        <v>20</v>
+      </c>
+      <c r="M158" s="3">
+        <v>21</v>
+      </c>
+      <c r="N158" s="3">
+        <v>23</v>
+      </c>
+      <c r="O158" s="3">
         <v>24</v>
       </c>
-      <c r="B158" s="3">
-        <v>3</v>
-      </c>
-      <c r="C158" s="3">
-        <v>4</v>
-      </c>
-      <c r="D158" s="3">
-        <v>5</v>
-      </c>
-      <c r="E158" s="3">
-        <v>8</v>
-      </c>
-      <c r="F158" s="3">
-        <v>9</v>
-      </c>
-      <c r="G158" s="3">
-        <v>10</v>
-      </c>
-      <c r="H158" s="3">
-        <v>11</v>
-      </c>
-      <c r="I158" s="3">
-        <v>12</v>
-      </c>
-      <c r="J158" s="3">
-        <v>13</v>
-      </c>
-      <c r="K158" s="3">
-        <v>15</v>
-      </c>
-      <c r="L158" s="3">
-        <v>16</v>
-      </c>
-      <c r="M158" s="3">
-        <v>18</v>
-      </c>
-      <c r="N158" s="3">
-        <v>19</v>
-      </c>
-      <c r="O158" s="3">
-        <v>21</v>
-      </c>
       <c r="P158" s="3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q158" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="R158" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="S158" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="T158" s="3">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="U158" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V158" s="3">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="W158" s="3">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="X158" s="3">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="Y158" s="3">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="Z158" s="3">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="AA158" s="3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="AB158" s="3">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="AC158" s="3">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="AD158" s="3">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="AE158" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AF158" s="3">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="AG158" s="3">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="AH158" s="3">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="AI158" s="3">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="AJ158" s="3"/>
       <c r="AK158" s="3"/>
       <c r="AL158" s="3"/>
-      <c r="AM158" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AM158" s="3"/>
       <c r="AN158" s="3"/>
       <c r="AO158" s="3"/>
       <c r="AP158" s="3"/>
@@ -55555,17 +55548,15 @@
       <c r="BE158" s="3"/>
       <c r="BF158" s="3"/>
       <c r="BG158" s="3"/>
-      <c r="BH158" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BH158" s="3"/>
       <c r="BI158" s="3"/>
       <c r="BJ158" s="3"/>
-      <c r="BK158" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK158" s="3"/>
       <c r="BL158" s="3"/>
       <c r="BM158" s="3"/>
-      <c r="BN158" s="3"/>
+      <c r="BN158" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BO158" s="3"/>
       <c r="BP158" s="3"/>
       <c r="BQ158" s="3"/>
@@ -55588,111 +55579,111 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="159" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B159" s="3">
+        <v>4</v>
+      </c>
+      <c r="C159" s="3">
+        <v>7</v>
+      </c>
+      <c r="D159" s="3">
+        <v>8</v>
+      </c>
+      <c r="E159" s="3">
+        <v>12</v>
+      </c>
+      <c r="F159" s="3">
+        <v>14</v>
+      </c>
+      <c r="G159" s="3">
+        <v>15</v>
+      </c>
+      <c r="H159" s="3">
+        <v>17</v>
+      </c>
+      <c r="I159" s="3">
+        <v>18</v>
+      </c>
+      <c r="J159" s="3">
+        <v>20</v>
+      </c>
+      <c r="K159" s="3">
+        <v>21</v>
+      </c>
+      <c r="L159" s="3">
+        <v>23</v>
+      </c>
+      <c r="M159" s="3">
+        <v>24</v>
+      </c>
+      <c r="N159" s="3">
+        <v>26</v>
+      </c>
+      <c r="O159" s="3">
         <v>27</v>
       </c>
-      <c r="B159" s="3">
-        <v>4</v>
-      </c>
-      <c r="C159" s="3">
-        <v>6</v>
-      </c>
-      <c r="D159" s="3">
-        <v>7</v>
-      </c>
-      <c r="E159" s="3">
-        <v>10</v>
-      </c>
-      <c r="F159" s="3">
-        <v>12</v>
-      </c>
-      <c r="G159" s="3">
-        <v>13</v>
-      </c>
-      <c r="H159" s="3">
-        <v>15</v>
-      </c>
-      <c r="I159" s="3">
-        <v>16</v>
-      </c>
-      <c r="J159" s="3">
-        <v>17</v>
-      </c>
-      <c r="K159" s="3">
-        <v>19</v>
-      </c>
-      <c r="L159" s="3">
-        <v>20</v>
-      </c>
-      <c r="M159" s="3">
-        <v>21</v>
-      </c>
-      <c r="N159" s="3">
-        <v>23</v>
-      </c>
-      <c r="O159" s="3">
-        <v>24</v>
-      </c>
       <c r="P159" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Q159" s="3">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="R159" s="3">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="S159" s="3">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="T159" s="3">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="U159" s="3">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="V159" s="3">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="W159" s="3">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="X159" s="3">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="Y159" s="3">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="Z159" s="3">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="AA159" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="AB159" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="AC159" s="3">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="AD159" s="3">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="AE159" s="3">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="AF159" s="3">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="AG159" s="3">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="AH159" s="3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AI159" s="3">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="AJ159" s="3"/>
       <c r="AK159" s="3"/>
@@ -55703,7 +55694,9 @@
       <c r="AP159" s="3"/>
       <c r="AQ159" s="3"/>
       <c r="AR159" s="3"/>
-      <c r="AS159" s="3"/>
+      <c r="AS159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AT159" s="3"/>
       <c r="AU159" s="3"/>
       <c r="AV159" s="3"/>
@@ -55714,20 +55707,28 @@
       <c r="BA159" s="3"/>
       <c r="BB159" s="3"/>
       <c r="BC159" s="3"/>
-      <c r="BD159" s="3"/>
+      <c r="BD159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BE159" s="3"/>
       <c r="BF159" s="3"/>
       <c r="BG159" s="3"/>
       <c r="BH159" s="3"/>
-      <c r="BI159" s="3"/>
+      <c r="BI159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BJ159" s="3"/>
-      <c r="BK159" s="3"/>
-      <c r="BL159" s="3"/>
+      <c r="BK159" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BM159" s="3"/>
-      <c r="BN159" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO159" s="3"/>
+      <c r="BN159" s="3"/>
+      <c r="BO159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BP159" s="3"/>
       <c r="BQ159" s="3"/>
       <c r="BR159" s="3"/>
@@ -55736,22 +55737,26 @@
       <c r="BU159" s="3"/>
       <c r="BV159" s="3"/>
       <c r="BW159" s="3"/>
-      <c r="BX159" s="3"/>
+      <c r="BX159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BY159" s="3"/>
       <c r="BZ159" s="3"/>
       <c r="CA159" s="3"/>
       <c r="CB159" s="3"/>
       <c r="CC159" s="3"/>
-      <c r="CD159" s="3"/>
+      <c r="CD159" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CE159" s="3"/>
       <c r="CF159" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="160" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B160" s="3">
         <v>4</v>
@@ -55921,12 +55926,12 @@
       <c r="CE160" s="3"/>
       <c r="CF160" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="161" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B161" s="3">
         <v>4</v>
@@ -56099,9 +56104,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="162" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="B162" s="3">
         <v>4</v>
@@ -56206,7 +56211,9 @@
         <v>57</v>
       </c>
       <c r="AJ162" s="3"/>
-      <c r="AK162" s="3"/>
+      <c r="AK162" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AL162" s="3"/>
       <c r="AM162" s="3"/>
       <c r="AN162" s="3"/>
@@ -56214,9 +56221,7 @@
       <c r="AP162" s="3"/>
       <c r="AQ162" s="3"/>
       <c r="AR162" s="3"/>
-      <c r="AS162" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AS162" s="3"/>
       <c r="AT162" s="3"/>
       <c r="AU162" s="3"/>
       <c r="AV162" s="3"/>
@@ -56227,20 +56232,18 @@
       <c r="BA162" s="3"/>
       <c r="BB162" s="3"/>
       <c r="BC162" s="3"/>
-      <c r="BD162" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BD162" s="3"/>
       <c r="BE162" s="3"/>
-      <c r="BF162" s="3"/>
+      <c r="BF162" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BG162" s="3"/>
       <c r="BH162" s="3"/>
       <c r="BI162" s="3" t="s">
         <v>63</v>
       </c>
       <c r="BJ162" s="3"/>
-      <c r="BK162" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK162" s="3"/>
       <c r="BL162" s="3" t="s">
         <v>63</v>
       </c>
@@ -56262,7 +56265,9 @@
       </c>
       <c r="BY162" s="3"/>
       <c r="BZ162" s="3"/>
-      <c r="CA162" s="3"/>
+      <c r="CA162" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CB162" s="3"/>
       <c r="CC162" s="3"/>
       <c r="CD162" s="3" t="s">
@@ -56274,9 +56279,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="163" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="B163" s="3">
         <v>4</v>
@@ -56381,9 +56386,7 @@
         <v>57</v>
       </c>
       <c r="AJ163" s="3"/>
-      <c r="AK163" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AK163" s="3"/>
       <c r="AL163" s="3"/>
       <c r="AM163" s="3"/>
       <c r="AN163" s="3"/>
@@ -56391,7 +56394,9 @@
       <c r="AP163" s="3"/>
       <c r="AQ163" s="3"/>
       <c r="AR163" s="3"/>
-      <c r="AS163" s="3"/>
+      <c r="AS163" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AT163" s="3"/>
       <c r="AU163" s="3"/>
       <c r="AV163" s="3"/>
@@ -56402,18 +56407,20 @@
       <c r="BA163" s="3"/>
       <c r="BB163" s="3"/>
       <c r="BC163" s="3"/>
-      <c r="BD163" s="3"/>
+      <c r="BD163" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BE163" s="3"/>
-      <c r="BF163" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF163" s="3"/>
       <c r="BG163" s="3"/>
       <c r="BH163" s="3"/>
       <c r="BI163" s="3" t="s">
         <v>63</v>
       </c>
       <c r="BJ163" s="3"/>
-      <c r="BK163" s="3"/>
+      <c r="BK163" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BL163" s="3" t="s">
         <v>63</v>
       </c>
@@ -56435,9 +56442,7 @@
       </c>
       <c r="BY163" s="3"/>
       <c r="BZ163" s="3"/>
-      <c r="CA163" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CA163" s="3"/>
       <c r="CB163" s="3"/>
       <c r="CC163" s="3"/>
       <c r="CD163" s="3" t="s">
@@ -56449,9 +56454,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="164" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B164" s="3">
         <v>4</v>
@@ -56624,9 +56629,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="165" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B165" s="3">
         <v>4</v>
@@ -56799,9 +56804,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="166" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B166" s="3">
         <v>4</v>
@@ -56974,9 +56979,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="167" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B167" s="3">
         <v>4</v>
@@ -57121,9 +57126,7 @@
       </c>
       <c r="BM167" s="3"/>
       <c r="BN167" s="3"/>
-      <c r="BO167" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BO167" s="3"/>
       <c r="BP167" s="3"/>
       <c r="BQ167" s="3"/>
       <c r="BR167" s="3"/>
@@ -57149,9 +57152,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="168" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="B168" s="3">
         <v>4</v>
@@ -57169,91 +57172,91 @@
         <v>14</v>
       </c>
       <c r="G168" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H168" s="3">
         <v>17</v>
       </c>
       <c r="I168" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J168" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K168" s="3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L168" s="3">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M168" s="3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N168" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O168" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P168" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q168" s="3">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R168" s="3">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S168" s="3">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="T168" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U168" s="3">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V168" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="W168" s="3">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="X168" s="3">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Y168" s="3">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Z168" s="3">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AA168" s="3">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AB168" s="3">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="AC168" s="3">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AD168" s="3">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="AE168" s="3">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AF168" s="3">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AG168" s="3">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AH168" s="3">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AI168" s="3">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AJ168" s="3"/>
       <c r="AK168" s="3"/>
@@ -57264,39 +57267,35 @@
       <c r="AP168" s="3"/>
       <c r="AQ168" s="3"/>
       <c r="AR168" s="3"/>
-      <c r="AS168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AS168" s="3"/>
       <c r="AT168" s="3"/>
       <c r="AU168" s="3"/>
       <c r="AV168" s="3"/>
-      <c r="AW168" s="3"/>
+      <c r="AW168" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AX168" s="3"/>
       <c r="AY168" s="3"/>
       <c r="AZ168" s="3"/>
       <c r="BA168" s="3"/>
       <c r="BB168" s="3"/>
       <c r="BC168" s="3"/>
-      <c r="BD168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BD168" s="3"/>
       <c r="BE168" s="3"/>
       <c r="BF168" s="3"/>
       <c r="BG168" s="3"/>
       <c r="BH168" s="3"/>
-      <c r="BI168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BI168" s="3"/>
       <c r="BJ168" s="3"/>
-      <c r="BK168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK168" s="3"/>
       <c r="BL168" s="3" t="s">
         <v>63</v>
       </c>
       <c r="BM168" s="3"/>
       <c r="BN168" s="3"/>
-      <c r="BO168" s="3"/>
+      <c r="BO168" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BP168" s="3"/>
       <c r="BQ168" s="3"/>
       <c r="BR168" s="3"/>
@@ -57305,26 +57304,22 @@
       <c r="BU168" s="3"/>
       <c r="BV168" s="3"/>
       <c r="BW168" s="3"/>
-      <c r="BX168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BX168" s="3"/>
       <c r="BY168" s="3"/>
       <c r="BZ168" s="3"/>
       <c r="CA168" s="3"/>
       <c r="CB168" s="3"/>
       <c r="CC168" s="3"/>
-      <c r="CD168" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CD168" s="3"/>
       <c r="CE168" s="3"/>
       <c r="CF168" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="169" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B169" s="3">
         <v>4</v>
@@ -57484,12 +57479,12 @@
       <c r="CE169" s="3"/>
       <c r="CF169" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="170" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B170" s="3">
         <v>4</v>
@@ -57652,111 +57647,111 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="171" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
       <c r="B171" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C171" s="3">
+        <v>6</v>
+      </c>
+      <c r="D171" s="3">
         <v>7</v>
       </c>
-      <c r="D171" s="3">
+      <c r="E171" s="3">
         <v>8</v>
       </c>
-      <c r="E171" s="3">
+      <c r="F171" s="3">
+        <v>9</v>
+      </c>
+      <c r="G171" s="3">
+        <v>9</v>
+      </c>
+      <c r="H171" s="3">
+        <v>10</v>
+      </c>
+      <c r="I171" s="3">
+        <v>10</v>
+      </c>
+      <c r="J171" s="3">
+        <v>11</v>
+      </c>
+      <c r="K171" s="3">
+        <v>11</v>
+      </c>
+      <c r="L171" s="3">
         <v>12</v>
       </c>
-      <c r="F171" s="3">
+      <c r="M171" s="3">
+        <v>12</v>
+      </c>
+      <c r="N171" s="3">
+        <v>13</v>
+      </c>
+      <c r="O171" s="3">
+        <v>13</v>
+      </c>
+      <c r="P171" s="3">
         <v>14</v>
       </c>
-      <c r="G171" s="3">
+      <c r="Q171" s="3">
+        <v>14</v>
+      </c>
+      <c r="R171" s="3">
+        <v>15</v>
+      </c>
+      <c r="S171" s="3">
+        <v>15</v>
+      </c>
+      <c r="T171" s="3">
         <v>16</v>
       </c>
-      <c r="H171" s="3">
+      <c r="U171" s="3">
+        <v>16</v>
+      </c>
+      <c r="V171" s="3">
         <v>17</v>
       </c>
-      <c r="I171" s="3">
+      <c r="W171" s="3">
+        <v>17</v>
+      </c>
+      <c r="X171" s="3">
+        <v>18</v>
+      </c>
+      <c r="Y171" s="3">
+        <v>18</v>
+      </c>
+      <c r="Z171" s="3">
         <v>19</v>
       </c>
-      <c r="J171" s="3">
+      <c r="AA171" s="3">
+        <v>19</v>
+      </c>
+      <c r="AB171" s="3">
+        <v>20</v>
+      </c>
+      <c r="AC171" s="3">
+        <v>20</v>
+      </c>
+      <c r="AD171" s="3">
         <v>21</v>
       </c>
-      <c r="K171" s="3">
+      <c r="AE171" s="3">
+        <v>21</v>
+      </c>
+      <c r="AF171" s="3">
         <v>22</v>
       </c>
-      <c r="L171" s="3">
-        <v>24</v>
-      </c>
-      <c r="M171" s="3">
-        <v>25</v>
-      </c>
-      <c r="N171" s="3">
-        <v>27</v>
-      </c>
-      <c r="O171" s="3">
-        <v>29</v>
-      </c>
-      <c r="P171" s="3">
-        <v>30</v>
-      </c>
-      <c r="Q171" s="3">
-        <v>32</v>
-      </c>
-      <c r="R171" s="3">
-        <v>33</v>
-      </c>
-      <c r="S171" s="3">
-        <v>35</v>
-      </c>
-      <c r="T171" s="3">
-        <v>37</v>
-      </c>
-      <c r="U171" s="3">
-        <v>38</v>
-      </c>
-      <c r="V171" s="3">
-        <v>40</v>
-      </c>
-      <c r="W171" s="3">
-        <v>41</v>
-      </c>
-      <c r="X171" s="3">
-        <v>43</v>
-      </c>
-      <c r="Y171" s="3">
-        <v>45</v>
-      </c>
-      <c r="Z171" s="3">
-        <v>46</v>
-      </c>
-      <c r="AA171" s="3">
-        <v>48</v>
-      </c>
-      <c r="AB171" s="3">
-        <v>49</v>
-      </c>
-      <c r="AC171" s="3">
-        <v>51</v>
-      </c>
-      <c r="AD171" s="3">
-        <v>53</v>
-      </c>
-      <c r="AE171" s="3">
-        <v>54</v>
-      </c>
-      <c r="AF171" s="3">
-        <v>56</v>
-      </c>
       <c r="AG171" s="3">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="AH171" s="3">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="AI171" s="3">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="AJ171" s="3"/>
       <c r="AK171" s="3"/>
@@ -57771,9 +57766,7 @@
       <c r="AT171" s="3"/>
       <c r="AU171" s="3"/>
       <c r="AV171" s="3"/>
-      <c r="AW171" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AW171" s="3"/>
       <c r="AX171" s="3"/>
       <c r="AY171" s="3"/>
       <c r="AZ171" s="3"/>
@@ -57784,42 +57777,50 @@
       <c r="BE171" s="3"/>
       <c r="BF171" s="3"/>
       <c r="BG171" s="3"/>
-      <c r="BH171" s="3"/>
+      <c r="BH171" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BI171" s="3"/>
       <c r="BJ171" s="3"/>
-      <c r="BK171" s="3"/>
-      <c r="BL171" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK171" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL171" s="3"/>
       <c r="BM171" s="3"/>
       <c r="BN171" s="3"/>
-      <c r="BO171" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BO171" s="3"/>
       <c r="BP171" s="3"/>
       <c r="BQ171" s="3"/>
-      <c r="BR171" s="3"/>
+      <c r="BR171" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BS171" s="3"/>
       <c r="BT171" s="3"/>
-      <c r="BU171" s="3"/>
+      <c r="BU171" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BV171" s="3"/>
       <c r="BW171" s="3"/>
       <c r="BX171" s="3"/>
       <c r="BY171" s="3"/>
-      <c r="BZ171" s="3"/>
+      <c r="BZ171" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CA171" s="3"/>
       <c r="CB171" s="3"/>
       <c r="CC171" s="3"/>
-      <c r="CD171" s="3"/>
+      <c r="CD171" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CE171" s="3"/>
       <c r="CF171" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="172" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B172" s="3">
         <v>6</v>
@@ -57985,12 +57986,12 @@
       <c r="CE172" s="3"/>
       <c r="CF172" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="173" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B173" s="3">
         <v>6</v>
@@ -58159,9 +58160,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="174" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B174" s="3">
         <v>6</v>
@@ -58330,9 +58331,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="175" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B175" s="3">
         <v>6</v>
@@ -58501,9 +58502,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="176" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B176" s="3">
         <v>6</v>
@@ -58672,9 +58673,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="177" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B177" s="3">
         <v>6</v>
@@ -58843,9 +58844,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="178" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B178" s="3">
         <v>6</v>
@@ -59014,9 +59015,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="179" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B179" s="3">
         <v>6</v>
@@ -59185,9 +59186,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="180" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B180" s="3">
         <v>6</v>
@@ -59356,111 +59357,111 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="181" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>243</v>
+        <v>13</v>
       </c>
       <c r="B181" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C181" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D181" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E181" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F181" s="3">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G181" s="3">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H181" s="3">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="I181" s="3">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J181" s="3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="K181" s="3">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="L181" s="3">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="M181" s="3">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="N181" s="3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="O181" s="3">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="P181" s="3">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="Q181" s="3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="R181" s="3">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="S181" s="3">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="T181" s="3">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="U181" s="3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="V181" s="3">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="W181" s="3">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="X181" s="3">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="Y181" s="3">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="Z181" s="3">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="AA181" s="3">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="AB181" s="3">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="AC181" s="3">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="AD181" s="3">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="AE181" s="3">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="AF181" s="3">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="AG181" s="3">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="AH181" s="3">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="AI181" s="3">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="AJ181" s="3"/>
       <c r="AK181" s="3"/>
@@ -59480,15 +59481,15 @@
       <c r="AY181" s="3"/>
       <c r="AZ181" s="3"/>
       <c r="BA181" s="3"/>
-      <c r="BB181" s="3"/>
+      <c r="BB181" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BC181" s="3"/>
       <c r="BD181" s="3"/>
       <c r="BE181" s="3"/>
       <c r="BF181" s="3"/>
       <c r="BG181" s="3"/>
-      <c r="BH181" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BH181" s="3"/>
       <c r="BI181" s="3"/>
       <c r="BJ181" s="3"/>
       <c r="BK181" s="3" t="s">
@@ -59512,126 +59513,122 @@
       <c r="BW181" s="3"/>
       <c r="BX181" s="3"/>
       <c r="BY181" s="3"/>
-      <c r="BZ181" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BZ181" s="3"/>
       <c r="CA181" s="3"/>
       <c r="CB181" s="3"/>
       <c r="CC181" s="3"/>
-      <c r="CD181" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CD181" s="3"/>
       <c r="CE181" s="3"/>
       <c r="CF181" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="182" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="B182" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C182" s="3">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D182" s="3">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E182" s="3">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F182" s="3">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G182" s="3">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="H182" s="3">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="I182" s="3">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="J182" s="3">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="K182" s="3">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="L182" s="3">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="M182" s="3">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="N182" s="3">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="O182" s="3">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="P182" s="3">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="Q182" s="3">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="R182" s="3">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="S182" s="3">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="T182" s="3">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="U182" s="3">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="V182" s="3">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="W182" s="3">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="X182" s="3">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="Y182" s="3">
-        <v>34</v>
+        <v>114</v>
       </c>
       <c r="Z182" s="3">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="AA182" s="3">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="AB182" s="3">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="AC182" s="3">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="AD182" s="3">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="AE182" s="3">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="AF182" s="3">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="AG182" s="3">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="AH182" s="3">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="AI182" s="3">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="AJ182" s="3"/>
       <c r="AK182" s="3"/>
@@ -59651,34 +59648,28 @@
       <c r="AY182" s="3"/>
       <c r="AZ182" s="3"/>
       <c r="BA182" s="3"/>
-      <c r="BB182" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BB182" s="3"/>
       <c r="BC182" s="3"/>
       <c r="BD182" s="3"/>
       <c r="BE182" s="3"/>
-      <c r="BF182" s="3"/>
+      <c r="BF182" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BG182" s="3"/>
       <c r="BH182" s="3"/>
       <c r="BI182" s="3"/>
       <c r="BJ182" s="3"/>
-      <c r="BK182" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK182" s="3"/>
       <c r="BL182" s="3"/>
       <c r="BM182" s="3"/>
       <c r="BN182" s="3"/>
       <c r="BO182" s="3"/>
       <c r="BP182" s="3"/>
       <c r="BQ182" s="3"/>
-      <c r="BR182" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BR182" s="3"/>
       <c r="BS182" s="3"/>
       <c r="BT182" s="3"/>
-      <c r="BU182" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BU182" s="3"/>
       <c r="BV182" s="3"/>
       <c r="BW182" s="3"/>
       <c r="BX182" s="3"/>
@@ -59694,111 +59685,111 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="183" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="B183" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C183" s="3">
+        <v>13</v>
+      </c>
+      <c r="D183" s="3">
+        <v>13</v>
+      </c>
+      <c r="E183" s="3">
+        <v>15</v>
+      </c>
+      <c r="F183" s="3">
         <v>16</v>
       </c>
-      <c r="D183" s="3">
+      <c r="G183" s="3">
+        <v>17</v>
+      </c>
+      <c r="H183" s="3">
+        <v>18</v>
+      </c>
+      <c r="I183" s="3">
+        <v>18</v>
+      </c>
+      <c r="J183" s="3">
+        <v>19</v>
+      </c>
+      <c r="K183" s="3">
         <v>20</v>
       </c>
-      <c r="E183" s="3">
+      <c r="L183" s="3">
+        <v>21</v>
+      </c>
+      <c r="M183" s="3">
+        <v>21</v>
+      </c>
+      <c r="N183" s="3">
+        <v>22</v>
+      </c>
+      <c r="O183" s="3">
+        <v>23</v>
+      </c>
+      <c r="P183" s="3">
+        <v>24</v>
+      </c>
+      <c r="Q183" s="3">
+        <v>24</v>
+      </c>
+      <c r="R183" s="3">
+        <v>25</v>
+      </c>
+      <c r="S183" s="3">
+        <v>26</v>
+      </c>
+      <c r="T183" s="3">
+        <v>27</v>
+      </c>
+      <c r="U183" s="3">
+        <v>27</v>
+      </c>
+      <c r="V183" s="3">
+        <v>28</v>
+      </c>
+      <c r="W183" s="3">
+        <v>29</v>
+      </c>
+      <c r="X183" s="3">
         <v>30</v>
       </c>
-      <c r="F183" s="3">
+      <c r="Y183" s="3">
+        <v>30</v>
+      </c>
+      <c r="Z183" s="3">
+        <v>31</v>
+      </c>
+      <c r="AA183" s="3">
+        <v>32</v>
+      </c>
+      <c r="AB183" s="3">
+        <v>33</v>
+      </c>
+      <c r="AC183" s="3">
+        <v>33</v>
+      </c>
+      <c r="AD183" s="3">
+        <v>34</v>
+      </c>
+      <c r="AE183" s="3">
         <v>35</v>
       </c>
-      <c r="G183" s="3">
-        <v>39</v>
-      </c>
-      <c r="H183" s="3">
-        <v>44</v>
-      </c>
-      <c r="I183" s="3">
-        <v>48</v>
-      </c>
-      <c r="J183" s="3">
-        <v>52</v>
-      </c>
-      <c r="K183" s="3">
-        <v>56</v>
-      </c>
-      <c r="L183" s="3">
-        <v>60</v>
-      </c>
-      <c r="M183" s="3">
-        <v>64</v>
-      </c>
-      <c r="N183" s="3">
-        <v>68</v>
-      </c>
-      <c r="O183" s="3">
-        <v>72</v>
-      </c>
-      <c r="P183" s="3">
-        <v>77</v>
-      </c>
-      <c r="Q183" s="3">
-        <v>81</v>
-      </c>
-      <c r="R183" s="3">
-        <v>85</v>
-      </c>
-      <c r="S183" s="3">
-        <v>89</v>
-      </c>
-      <c r="T183" s="3">
-        <v>93</v>
-      </c>
-      <c r="U183" s="3">
-        <v>97</v>
-      </c>
-      <c r="V183" s="3">
-        <v>101</v>
-      </c>
-      <c r="W183" s="3">
-        <v>105</v>
-      </c>
-      <c r="X183" s="3">
-        <v>110</v>
-      </c>
-      <c r="Y183" s="3">
-        <v>114</v>
-      </c>
-      <c r="Z183" s="3">
-        <v>118</v>
-      </c>
-      <c r="AA183" s="3">
-        <v>122</v>
-      </c>
-      <c r="AB183" s="3">
-        <v>126</v>
-      </c>
-      <c r="AC183" s="3">
-        <v>130</v>
-      </c>
-      <c r="AD183" s="3">
-        <v>134</v>
-      </c>
-      <c r="AE183" s="3">
-        <v>138</v>
-      </c>
       <c r="AF183" s="3">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="AG183" s="3">
-        <v>147</v>
+        <v>36</v>
       </c>
       <c r="AH183" s="3">
-        <v>151</v>
+        <v>37</v>
       </c>
       <c r="AI183" s="3">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="AJ183" s="3"/>
       <c r="AK183" s="3"/>
@@ -59810,7 +59801,9 @@
       <c r="AQ183" s="3"/>
       <c r="AR183" s="3"/>
       <c r="AS183" s="3"/>
-      <c r="AT183" s="3"/>
+      <c r="AT183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AU183" s="3"/>
       <c r="AV183" s="3"/>
       <c r="AW183" s="3"/>
@@ -59822,17 +59815,23 @@
       <c r="BC183" s="3"/>
       <c r="BD183" s="3"/>
       <c r="BE183" s="3"/>
-      <c r="BF183" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF183" s="3"/>
       <c r="BG183" s="3"/>
-      <c r="BH183" s="3"/>
+      <c r="BH183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BI183" s="3"/>
       <c r="BJ183" s="3"/>
-      <c r="BK183" s="3"/>
-      <c r="BL183" s="3"/>
+      <c r="BK183" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BM183" s="3"/>
-      <c r="BN183" s="3"/>
+      <c r="BN183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BO183" s="3"/>
       <c r="BP183" s="3"/>
       <c r="BQ183" s="3"/>
@@ -59841,13 +59840,19 @@
       <c r="BT183" s="3"/>
       <c r="BU183" s="3"/>
       <c r="BV183" s="3"/>
-      <c r="BW183" s="3"/>
+      <c r="BW183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BX183" s="3"/>
       <c r="BY183" s="3"/>
-      <c r="BZ183" s="3"/>
+      <c r="BZ183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CA183" s="3"/>
       <c r="CB183" s="3"/>
-      <c r="CC183" s="3"/>
+      <c r="CC183" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CD183" s="3"/>
       <c r="CE183" s="3"/>
       <c r="CF183" s="1" t="str">
@@ -59855,9 +59860,9 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="184" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B184" s="3">
         <v>11</v>
@@ -60027,12 +60032,12 @@
       <c r="CE184" s="3"/>
       <c r="CF184" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="185" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B185" s="3">
         <v>11</v>
@@ -60205,9 +60210,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="186" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B186" s="3">
         <v>11</v>
@@ -60380,9 +60385,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="187" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B187" s="3">
         <v>11</v>
@@ -60555,111 +60560,111 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="188" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="B188" s="3">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C188" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D188" s="3">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E188" s="3">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F188" s="3">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="G188" s="3">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="H188" s="3">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I188" s="3">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="J188" s="3">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="K188" s="3">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="L188" s="3">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="M188" s="3">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="N188" s="3">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="O188" s="3">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="P188" s="3">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="Q188" s="3">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="R188" s="3">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="S188" s="3">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="T188" s="3">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="U188" s="3">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="V188" s="3">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="W188" s="3">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="X188" s="3">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="Y188" s="3">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="Z188" s="3">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="AA188" s="3">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="AB188" s="3">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="AC188" s="3">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="AD188" s="3">
-        <v>34</v>
+        <v>98</v>
       </c>
       <c r="AE188" s="3">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="AF188" s="3">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="AG188" s="3">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="AH188" s="3">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="AI188" s="3">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="AJ188" s="3"/>
       <c r="AK188" s="3"/>
@@ -60671,12 +60676,12 @@
       <c r="AQ188" s="3"/>
       <c r="AR188" s="3"/>
       <c r="AS188" s="3"/>
-      <c r="AT188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AT188" s="3"/>
       <c r="AU188" s="3"/>
       <c r="AV188" s="3"/>
-      <c r="AW188" s="3"/>
+      <c r="AW188" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AX188" s="3"/>
       <c r="AY188" s="3"/>
       <c r="AZ188" s="3"/>
@@ -60687,21 +60692,15 @@
       <c r="BE188" s="3"/>
       <c r="BF188" s="3"/>
       <c r="BG188" s="3"/>
-      <c r="BH188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BH188" s="3"/>
       <c r="BI188" s="3"/>
       <c r="BJ188" s="3"/>
-      <c r="BK188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK188" s="3"/>
       <c r="BL188" s="3" t="s">
         <v>63</v>
       </c>
       <c r="BM188" s="3"/>
-      <c r="BN188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BN188" s="3"/>
       <c r="BO188" s="3"/>
       <c r="BP188" s="3"/>
       <c r="BQ188" s="3"/>
@@ -60710,131 +60709,125 @@
       <c r="BT188" s="3"/>
       <c r="BU188" s="3"/>
       <c r="BV188" s="3"/>
-      <c r="BW188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BW188" s="3"/>
       <c r="BX188" s="3"/>
       <c r="BY188" s="3"/>
-      <c r="BZ188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BZ188" s="3"/>
       <c r="CA188" s="3"/>
       <c r="CB188" s="3"/>
-      <c r="CC188" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CC188" s="3"/>
       <c r="CD188" s="3"/>
       <c r="CE188" s="3"/>
       <c r="CF188" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="189" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="B189" s="3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C189" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D189" s="3">
         <v>23</v>
       </c>
       <c r="E189" s="3">
+        <v>27</v>
+      </c>
+      <c r="F189" s="3">
         <v>29</v>
       </c>
-      <c r="F189" s="3">
+      <c r="G189" s="3">
+        <v>31</v>
+      </c>
+      <c r="H189" s="3">
         <v>33</v>
       </c>
-      <c r="G189" s="3">
+      <c r="I189" s="3">
+        <v>35</v>
+      </c>
+      <c r="J189" s="3">
         <v>36</v>
       </c>
-      <c r="H189" s="3">
+      <c r="K189" s="3">
         <v>38</v>
       </c>
-      <c r="I189" s="3">
-        <v>41</v>
-      </c>
-      <c r="J189" s="3">
-        <v>44</v>
-      </c>
-      <c r="K189" s="3">
-        <v>46</v>
-      </c>
       <c r="L189" s="3">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="M189" s="3">
+        <v>42</v>
+      </c>
+      <c r="N189" s="3">
+        <v>43</v>
+      </c>
+      <c r="O189" s="3">
+        <v>45</v>
+      </c>
+      <c r="P189" s="3">
+        <v>47</v>
+      </c>
+      <c r="Q189" s="3">
+        <v>48</v>
+      </c>
+      <c r="R189" s="3">
+        <v>50</v>
+      </c>
+      <c r="S189" s="3">
         <v>52</v>
       </c>
-      <c r="N189" s="3">
+      <c r="T189" s="3">
+        <v>54</v>
+      </c>
+      <c r="U189" s="3">
         <v>55</v>
       </c>
-      <c r="O189" s="3">
+      <c r="V189" s="3">
         <v>57</v>
       </c>
-      <c r="P189" s="3">
-        <v>60</v>
-      </c>
-      <c r="Q189" s="3">
-        <v>63</v>
-      </c>
-      <c r="R189" s="3">
-        <v>65</v>
-      </c>
-      <c r="S189" s="3">
-        <v>68</v>
-      </c>
-      <c r="T189" s="3">
+      <c r="W189" s="3">
+        <v>59</v>
+      </c>
+      <c r="X189" s="3">
+        <v>61</v>
+      </c>
+      <c r="Y189" s="3">
+        <v>62</v>
+      </c>
+      <c r="Z189" s="3">
+        <v>64</v>
+      </c>
+      <c r="AA189" s="3">
+        <v>66</v>
+      </c>
+      <c r="AB189" s="3">
+        <v>67</v>
+      </c>
+      <c r="AC189" s="3">
+        <v>69</v>
+      </c>
+      <c r="AD189" s="3">
         <v>71</v>
       </c>
-      <c r="U189" s="3">
+      <c r="AE189" s="3">
         <v>73</v>
       </c>
-      <c r="V189" s="3">
+      <c r="AF189" s="3">
+        <v>74</v>
+      </c>
+      <c r="AG189" s="3">
         <v>76</v>
       </c>
-      <c r="W189" s="3">
+      <c r="AH189" s="3">
+        <v>78</v>
+      </c>
+      <c r="AI189" s="3">
         <v>79</v>
-      </c>
-      <c r="X189" s="3">
-        <v>82</v>
-      </c>
-      <c r="Y189" s="3">
-        <v>84</v>
-      </c>
-      <c r="Z189" s="3">
-        <v>87</v>
-      </c>
-      <c r="AA189" s="3">
-        <v>90</v>
-      </c>
-      <c r="AB189" s="3">
-        <v>92</v>
-      </c>
-      <c r="AC189" s="3">
-        <v>95</v>
-      </c>
-      <c r="AD189" s="3">
-        <v>98</v>
-      </c>
-      <c r="AE189" s="3">
-        <v>100</v>
-      </c>
-      <c r="AF189" s="3">
-        <v>103</v>
-      </c>
-      <c r="AG189" s="3">
-        <v>106</v>
-      </c>
-      <c r="AH189" s="3">
-        <v>109</v>
-      </c>
-      <c r="AI189" s="3">
-        <v>111</v>
       </c>
       <c r="AJ189" s="3"/>
       <c r="AK189" s="3"/>
@@ -60849,10 +60842,10 @@
       <c r="AT189" s="3"/>
       <c r="AU189" s="3"/>
       <c r="AV189" s="3"/>
-      <c r="AW189" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AX189" s="3"/>
+      <c r="AW189" s="3"/>
+      <c r="AX189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AY189" s="3"/>
       <c r="AZ189" s="3"/>
       <c r="BA189" s="3"/>
@@ -60866,36 +60859,44 @@
       <c r="BI189" s="3"/>
       <c r="BJ189" s="3"/>
       <c r="BK189" s="3"/>
-      <c r="BL189" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM189" s="3"/>
+      <c r="BL189" s="3"/>
+      <c r="BM189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BN189" s="3"/>
       <c r="BO189" s="3"/>
       <c r="BP189" s="3"/>
       <c r="BQ189" s="3"/>
-      <c r="BR189" s="3"/>
+      <c r="BR189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BS189" s="3"/>
       <c r="BT189" s="3"/>
-      <c r="BU189" s="3"/>
+      <c r="BU189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BV189" s="3"/>
       <c r="BW189" s="3"/>
       <c r="BX189" s="3"/>
       <c r="BY189" s="3"/>
       <c r="BZ189" s="3"/>
       <c r="CA189" s="3"/>
-      <c r="CB189" s="3"/>
+      <c r="CB189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CC189" s="3"/>
-      <c r="CD189" s="3"/>
+      <c r="CD189" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CE189" s="3"/>
       <c r="CF189" s="1" t="str">
         <f t="shared" si="2"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="190" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B190" s="3">
         <v>19</v>
@@ -61061,12 +61062,12 @@
       <c r="CE190" s="3"/>
       <c r="CF190" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="191" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B191" s="3">
         <v>19</v>
@@ -61226,18 +61227,16 @@
         <v>63</v>
       </c>
       <c r="CC191" s="3"/>
-      <c r="CD191" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CD191" s="3"/>
       <c r="CE191" s="3"/>
       <c r="CF191" s="1" t="str">
         <f t="shared" si="2"/>
         <v>YES</v>
       </c>
     </row>
-    <row r="192" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="B192" s="3">
         <v>19</v>
@@ -61346,24 +61345,28 @@
       <c r="AL192" s="3"/>
       <c r="AM192" s="3"/>
       <c r="AN192" s="3"/>
-      <c r="AO192" s="3"/>
+      <c r="AO192" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AP192" s="3"/>
       <c r="AQ192" s="3"/>
-      <c r="AR192" s="3"/>
+      <c r="AR192" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AS192" s="3"/>
       <c r="AT192" s="3"/>
       <c r="AU192" s="3"/>
       <c r="AV192" s="3"/>
       <c r="AW192" s="3"/>
-      <c r="AX192" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AX192" s="3"/>
       <c r="AY192" s="3"/>
       <c r="AZ192" s="3"/>
       <c r="BA192" s="3"/>
       <c r="BB192" s="3"/>
       <c r="BC192" s="3"/>
-      <c r="BD192" s="3"/>
+      <c r="BD192" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BE192" s="3"/>
       <c r="BF192" s="3"/>
       <c r="BG192" s="3"/>
@@ -61379,23 +61382,17 @@
       <c r="BO192" s="3"/>
       <c r="BP192" s="3"/>
       <c r="BQ192" s="3"/>
-      <c r="BR192" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BR192" s="3"/>
       <c r="BS192" s="3"/>
       <c r="BT192" s="3"/>
-      <c r="BU192" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BU192" s="3"/>
       <c r="BV192" s="3"/>
       <c r="BW192" s="3"/>
       <c r="BX192" s="3"/>
       <c r="BY192" s="3"/>
       <c r="BZ192" s="3"/>
       <c r="CA192" s="3"/>
-      <c r="CB192" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CB192" s="3"/>
       <c r="CC192" s="3"/>
       <c r="CD192" s="3"/>
       <c r="CE192" s="3"/>
@@ -61404,9 +61401,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="193" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
       <c r="B193" s="3">
         <v>19</v>
@@ -61515,28 +61512,24 @@
       <c r="AL193" s="3"/>
       <c r="AM193" s="3"/>
       <c r="AN193" s="3"/>
-      <c r="AO193" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AO193" s="3"/>
       <c r="AP193" s="3"/>
       <c r="AQ193" s="3"/>
-      <c r="AR193" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AR193" s="3"/>
       <c r="AS193" s="3"/>
       <c r="AT193" s="3"/>
       <c r="AU193" s="3"/>
       <c r="AV193" s="3"/>
       <c r="AW193" s="3"/>
-      <c r="AX193" s="3"/>
+      <c r="AX193" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AY193" s="3"/>
       <c r="AZ193" s="3"/>
       <c r="BA193" s="3"/>
       <c r="BB193" s="3"/>
       <c r="BC193" s="3"/>
-      <c r="BD193" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BD193" s="3"/>
       <c r="BE193" s="3"/>
       <c r="BF193" s="3"/>
       <c r="BG193" s="3"/>
@@ -61552,28 +61545,36 @@
       <c r="BO193" s="3"/>
       <c r="BP193" s="3"/>
       <c r="BQ193" s="3"/>
-      <c r="BR193" s="3"/>
+      <c r="BR193" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BS193" s="3"/>
       <c r="BT193" s="3"/>
-      <c r="BU193" s="3"/>
+      <c r="BU193" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BV193" s="3"/>
       <c r="BW193" s="3"/>
       <c r="BX193" s="3"/>
       <c r="BY193" s="3"/>
       <c r="BZ193" s="3"/>
       <c r="CA193" s="3"/>
-      <c r="CB193" s="3"/>
+      <c r="CB193" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CC193" s="3"/>
-      <c r="CD193" s="3"/>
+      <c r="CD193" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CE193" s="3"/>
       <c r="CF193" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="CF193:CF211" si="3">IF(AND(B193=B192,C193=C192,D193=D192,E193=E192,F193=F192,G193=G192,H193=H192,I193=I192,J193=J192,K193=K192,L193=L192,M193=M192,N193=N192,O193=O192,P193=P192,Q193=Q192,R193=R192,S193=S192,T193=T192,U193=U192,V193=V192,W193=W192,X193=X192,Y193=Y192,Z193=Z192,AA193=AA192,AB193=AB192,AC193=AC192,AD193=AD192,AE193=AE192,AF193=AF192,AG193=AG192,AH193=AH192,AI193=AI192),"YES","NO")</f>
         <v>YES</v>
       </c>
     </row>
-    <row r="194" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B194" s="3">
         <v>19</v>
@@ -61738,13 +61739,13 @@
       </c>
       <c r="CE194" s="3"/>
       <c r="CF194" s="1" t="str">
-        <f t="shared" ref="CF194:CF212" si="3">IF(AND(B194=B193,C194=C193,D194=D193,E194=E193,F194=F193,G194=G193,H194=H193,I194=I193,J194=J193,K194=K193,L194=L193,M194=M193,N194=N193,O194=O193,P194=P193,Q194=Q193,R194=R193,S194=S193,T194=T193,U194=U193,V194=V193,W194=W193,X194=X193,Y194=Y193,Z194=Z193,AA194=AA193,AB194=AB193,AC194=AC193,AD194=AD193,AE194=AE193,AF194=AF193,AG194=AG193,AH194=AH193,AI194=AI193),"YES","NO")</f>
+        <f t="shared" si="3"/>
         <v>YES</v>
       </c>
     </row>
-    <row r="195" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B195" s="3">
         <v>19</v>
@@ -61913,9 +61914,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="196" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B196" s="3">
         <v>19</v>
@@ -62084,9 +62085,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="197" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B197" s="3">
         <v>19</v>
@@ -62255,9 +62256,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="198" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B198" s="3">
         <v>19</v>
@@ -62426,9 +62427,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="199" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B199" s="3">
         <v>19</v>
@@ -62597,111 +62598,111 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="200" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>209</v>
+        <v>28</v>
       </c>
       <c r="B200" s="3">
         <v>19</v>
       </c>
       <c r="C200" s="3">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D200" s="3">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E200" s="3">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="F200" s="3">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="G200" s="3">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="H200" s="3">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="I200" s="3">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="J200" s="3">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="K200" s="3">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="L200" s="3">
-        <v>40</v>
+        <v>121</v>
       </c>
       <c r="M200" s="3">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="N200" s="3">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="O200" s="3">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="P200" s="3">
-        <v>47</v>
+        <v>154</v>
       </c>
       <c r="Q200" s="3">
-        <v>48</v>
+        <v>162</v>
       </c>
       <c r="R200" s="3">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="S200" s="3">
-        <v>52</v>
+        <v>178</v>
       </c>
       <c r="T200" s="3">
-        <v>54</v>
+        <v>187</v>
       </c>
       <c r="U200" s="3">
-        <v>55</v>
+        <v>195</v>
       </c>
       <c r="V200" s="3">
-        <v>57</v>
+        <v>203</v>
       </c>
       <c r="W200" s="3">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="X200" s="3">
-        <v>61</v>
+        <v>220</v>
       </c>
       <c r="Y200" s="3">
-        <v>62</v>
+        <v>228</v>
       </c>
       <c r="Z200" s="3">
-        <v>64</v>
+        <v>236</v>
       </c>
       <c r="AA200" s="3">
-        <v>66</v>
+        <v>244</v>
       </c>
       <c r="AB200" s="3">
-        <v>67</v>
+        <v>253</v>
       </c>
       <c r="AC200" s="3">
-        <v>69</v>
+        <v>261</v>
       </c>
       <c r="AD200" s="3">
-        <v>71</v>
+        <v>269</v>
       </c>
       <c r="AE200" s="3">
-        <v>73</v>
+        <v>277</v>
       </c>
       <c r="AF200" s="3">
-        <v>74</v>
+        <v>286</v>
       </c>
       <c r="AG200" s="3">
-        <v>76</v>
+        <v>294</v>
       </c>
       <c r="AH200" s="3">
-        <v>78</v>
+        <v>302</v>
       </c>
       <c r="AI200" s="3">
-        <v>79</v>
+        <v>310</v>
       </c>
       <c r="AJ200" s="3"/>
       <c r="AK200" s="3"/>
@@ -62715,49 +62716,51 @@
       <c r="AS200" s="3"/>
       <c r="AT200" s="3"/>
       <c r="AU200" s="3"/>
-      <c r="AV200" s="3"/>
+      <c r="AV200" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AW200" s="3"/>
-      <c r="AX200" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AX200" s="3"/>
       <c r="AY200" s="3"/>
       <c r="AZ200" s="3"/>
       <c r="BA200" s="3"/>
-      <c r="BB200" s="3"/>
+      <c r="BB200" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BC200" s="3"/>
       <c r="BD200" s="3"/>
       <c r="BE200" s="3"/>
       <c r="BF200" s="3"/>
       <c r="BG200" s="3"/>
-      <c r="BH200" s="3"/>
+      <c r="BH200" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BI200" s="3"/>
       <c r="BJ200" s="3"/>
-      <c r="BK200" s="3"/>
-      <c r="BL200" s="3"/>
-      <c r="BM200" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BK200" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL200" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM200" s="3"/>
       <c r="BN200" s="3"/>
       <c r="BO200" s="3"/>
       <c r="BP200" s="3"/>
       <c r="BQ200" s="3"/>
-      <c r="BR200" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BR200" s="3"/>
       <c r="BS200" s="3"/>
       <c r="BT200" s="3"/>
-      <c r="BU200" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BU200" s="3"/>
       <c r="BV200" s="3"/>
       <c r="BW200" s="3"/>
-      <c r="BX200" s="3"/>
+      <c r="BX200" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BY200" s="3"/>
       <c r="BZ200" s="3"/>
       <c r="CA200" s="3"/>
-      <c r="CB200" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CB200" s="3"/>
       <c r="CC200" s="3"/>
       <c r="CD200" s="3" t="s">
         <v>63</v>
@@ -62765,114 +62768,114 @@
       <c r="CE200" s="3"/>
       <c r="CF200" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>YES</v>
+        <v>NO</v>
       </c>
     </row>
-    <row r="201" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>28</v>
+        <v>183</v>
       </c>
       <c r="B201" s="3">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C201" s="3">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D201" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E201" s="3">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F201" s="3">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G201" s="3">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="H201" s="3">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="I201" s="3">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="J201" s="3">
+        <v>73</v>
+      </c>
+      <c r="K201" s="3">
+        <v>77</v>
+      </c>
+      <c r="L201" s="3">
+        <v>80</v>
+      </c>
+      <c r="M201" s="3">
+        <v>84</v>
+      </c>
+      <c r="N201" s="3">
+        <v>87</v>
+      </c>
+      <c r="O201" s="3">
+        <v>90</v>
+      </c>
+      <c r="P201" s="3">
+        <v>94</v>
+      </c>
+      <c r="Q201" s="3">
+        <v>97</v>
+      </c>
+      <c r="R201" s="3">
+        <v>101</v>
+      </c>
+      <c r="S201" s="3">
         <v>104</v>
       </c>
-      <c r="K201" s="3">
-        <v>112</v>
-      </c>
-      <c r="L201" s="3">
-        <v>121</v>
-      </c>
-      <c r="M201" s="3">
-        <v>129</v>
-      </c>
-      <c r="N201" s="3">
-        <v>137</v>
-      </c>
-      <c r="O201" s="3">
-        <v>145</v>
-      </c>
-      <c r="P201" s="3">
-        <v>154</v>
-      </c>
-      <c r="Q201" s="3">
-        <v>162</v>
-      </c>
-      <c r="R201" s="3">
-        <v>170</v>
-      </c>
-      <c r="S201" s="3">
-        <v>178</v>
-      </c>
       <c r="T201" s="3">
-        <v>187</v>
+        <v>108</v>
       </c>
       <c r="U201" s="3">
-        <v>195</v>
+        <v>111</v>
       </c>
       <c r="V201" s="3">
-        <v>203</v>
+        <v>115</v>
       </c>
       <c r="W201" s="3">
-        <v>211</v>
+        <v>118</v>
       </c>
       <c r="X201" s="3">
-        <v>220</v>
+        <v>122</v>
       </c>
       <c r="Y201" s="3">
-        <v>228</v>
+        <v>125</v>
       </c>
       <c r="Z201" s="3">
-        <v>236</v>
+        <v>128</v>
       </c>
       <c r="AA201" s="3">
-        <v>244</v>
+        <v>132</v>
       </c>
       <c r="AB201" s="3">
-        <v>253</v>
+        <v>135</v>
       </c>
       <c r="AC201" s="3">
-        <v>261</v>
+        <v>139</v>
       </c>
       <c r="AD201" s="3">
-        <v>269</v>
+        <v>142</v>
       </c>
       <c r="AE201" s="3">
-        <v>277</v>
+        <v>146</v>
       </c>
       <c r="AF201" s="3">
-        <v>286</v>
+        <v>149</v>
       </c>
       <c r="AG201" s="3">
-        <v>294</v>
+        <v>153</v>
       </c>
       <c r="AH201" s="3">
-        <v>302</v>
+        <v>156</v>
       </c>
       <c r="AI201" s="3">
-        <v>310</v>
+        <v>159</v>
       </c>
       <c r="AJ201" s="3"/>
       <c r="AK201" s="3"/>
@@ -62894,18 +62897,18 @@
       <c r="AY201" s="3"/>
       <c r="AZ201" s="3"/>
       <c r="BA201" s="3"/>
-      <c r="BB201" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BB201" s="3"/>
       <c r="BC201" s="3"/>
       <c r="BD201" s="3"/>
       <c r="BE201" s="3"/>
-      <c r="BF201" s="3"/>
+      <c r="BF201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BG201" s="3"/>
-      <c r="BH201" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI201" s="3"/>
+      <c r="BH201" s="3"/>
+      <c r="BI201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BJ201" s="3"/>
       <c r="BK201" s="3" t="s">
         <v>63</v>
@@ -62914,36 +62917,44 @@
         <v>63</v>
       </c>
       <c r="BM201" s="3"/>
-      <c r="BN201" s="3"/>
+      <c r="BN201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BO201" s="3"/>
       <c r="BP201" s="3"/>
-      <c r="BQ201" s="3"/>
+      <c r="BQ201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BR201" s="3"/>
       <c r="BS201" s="3"/>
-      <c r="BT201" s="3"/>
+      <c r="BT201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BU201" s="3"/>
       <c r="BV201" s="3"/>
-      <c r="BW201" s="3"/>
-      <c r="BX201" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BW201" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX201" s="3"/>
       <c r="BY201" s="3"/>
       <c r="BZ201" s="3"/>
-      <c r="CA201" s="3"/>
+      <c r="CA201" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CB201" s="3"/>
-      <c r="CC201" s="3"/>
-      <c r="CD201" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CC201" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="CD201" s="3"/>
       <c r="CE201" s="3"/>
       <c r="CF201" s="1" t="str">
         <f t="shared" si="3"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="202" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B202" s="3">
         <v>38</v>
@@ -63119,12 +63130,12 @@
       <c r="CE202" s="3"/>
       <c r="CF202" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
     </row>
-    <row r="203" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B203" s="3">
         <v>38</v>
@@ -63303,9 +63314,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="204" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>185</v>
+        <v>12</v>
       </c>
       <c r="B204" s="3">
         <v>38</v>
@@ -63416,31 +63427,29 @@
       <c r="AN204" s="3"/>
       <c r="AO204" s="3"/>
       <c r="AP204" s="3"/>
-      <c r="AQ204" s="3"/>
+      <c r="AQ204" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AR204" s="3"/>
       <c r="AS204" s="3"/>
       <c r="AT204" s="3"/>
       <c r="AU204" s="3"/>
-      <c r="AV204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AV204" s="3"/>
       <c r="AW204" s="3"/>
       <c r="AX204" s="3"/>
       <c r="AY204" s="3"/>
       <c r="AZ204" s="3"/>
       <c r="BA204" s="3"/>
-      <c r="BB204" s="3"/>
+      <c r="BB204" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BC204" s="3"/>
       <c r="BD204" s="3"/>
       <c r="BE204" s="3"/>
-      <c r="BF204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF204" s="3"/>
       <c r="BG204" s="3"/>
       <c r="BH204" s="3"/>
-      <c r="BI204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BI204" s="3"/>
       <c r="BJ204" s="3"/>
       <c r="BK204" s="3" t="s">
         <v>63</v>
@@ -63454,14 +63463,10 @@
       </c>
       <c r="BO204" s="3"/>
       <c r="BP204" s="3"/>
-      <c r="BQ204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BQ204" s="3"/>
       <c r="BR204" s="3"/>
       <c r="BS204" s="3"/>
-      <c r="BT204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BT204" s="3"/>
       <c r="BU204" s="3"/>
       <c r="BV204" s="3"/>
       <c r="BW204" s="3" t="s">
@@ -63470,13 +63475,9 @@
       <c r="BX204" s="3"/>
       <c r="BY204" s="3"/>
       <c r="BZ204" s="3"/>
-      <c r="CA204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CA204" s="3"/>
       <c r="CB204" s="3"/>
-      <c r="CC204" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="CC204" s="3"/>
       <c r="CD204" s="3"/>
       <c r="CE204" s="3"/>
       <c r="CF204" s="1" t="str">
@@ -63484,9 +63485,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="205" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="B205" s="3">
         <v>38</v>
@@ -63597,29 +63598,31 @@
       <c r="AN205" s="3"/>
       <c r="AO205" s="3"/>
       <c r="AP205" s="3"/>
-      <c r="AQ205" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="AQ205" s="3"/>
       <c r="AR205" s="3"/>
       <c r="AS205" s="3"/>
       <c r="AT205" s="3"/>
       <c r="AU205" s="3"/>
-      <c r="AV205" s="3"/>
+      <c r="AV205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="AW205" s="3"/>
       <c r="AX205" s="3"/>
       <c r="AY205" s="3"/>
       <c r="AZ205" s="3"/>
       <c r="BA205" s="3"/>
-      <c r="BB205" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="BB205" s="3"/>
       <c r="BC205" s="3"/>
       <c r="BD205" s="3"/>
       <c r="BE205" s="3"/>
-      <c r="BF205" s="3"/>
+      <c r="BF205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BG205" s="3"/>
       <c r="BH205" s="3"/>
-      <c r="BI205" s="3"/>
+      <c r="BI205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BJ205" s="3"/>
       <c r="BK205" s="3" t="s">
         <v>63</v>
@@ -63633,10 +63636,14 @@
       </c>
       <c r="BO205" s="3"/>
       <c r="BP205" s="3"/>
-      <c r="BQ205" s="3"/>
+      <c r="BQ205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BR205" s="3"/>
       <c r="BS205" s="3"/>
-      <c r="BT205" s="3"/>
+      <c r="BT205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BU205" s="3"/>
       <c r="BV205" s="3"/>
       <c r="BW205" s="3" t="s">
@@ -63645,9 +63652,13 @@
       <c r="BX205" s="3"/>
       <c r="BY205" s="3"/>
       <c r="BZ205" s="3"/>
-      <c r="CA205" s="3"/>
+      <c r="CA205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CB205" s="3"/>
-      <c r="CC205" s="3"/>
+      <c r="CC205" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="CD205" s="3"/>
       <c r="CE205" s="3"/>
       <c r="CF205" s="1" t="str">
@@ -63655,9 +63666,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="206" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B206" s="3">
         <v>38</v>
@@ -63836,9 +63847,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="207" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B207" s="3">
         <v>38</v>
@@ -64017,9 +64028,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="208" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B208" s="3">
         <v>38</v>
@@ -64198,9 +64209,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="209" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B209" s="3">
         <v>38</v>
@@ -64379,9 +64390,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="210" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B210" s="3">
         <v>38</v>
@@ -64560,9 +64571,9 @@
         <v>YES</v>
       </c>
     </row>
-    <row r="211" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B211" s="3">
         <v>38</v>
@@ -64709,7 +64720,9 @@
       <c r="BN211" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BO211" s="3"/>
+      <c r="BO211" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="BP211" s="3"/>
       <c r="BQ211" s="3" t="s">
         <v>63</v>
@@ -64737,189 +64750,6 @@
       <c r="CD211" s="3"/>
       <c r="CE211" s="3"/>
       <c r="CF211" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>YES</v>
-      </c>
-    </row>
-    <row r="212" spans="1:84" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A212" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B212" s="3">
-        <v>38</v>
-      </c>
-      <c r="C212" s="3">
-        <v>43</v>
-      </c>
-      <c r="D212" s="3">
-        <v>47</v>
-      </c>
-      <c r="E212" s="3">
-        <v>55</v>
-      </c>
-      <c r="F212" s="3">
-        <v>59</v>
-      </c>
-      <c r="G212" s="3">
-        <v>63</v>
-      </c>
-      <c r="H212" s="3">
-        <v>66</v>
-      </c>
-      <c r="I212" s="3">
-        <v>70</v>
-      </c>
-      <c r="J212" s="3">
-        <v>73</v>
-      </c>
-      <c r="K212" s="3">
-        <v>77</v>
-      </c>
-      <c r="L212" s="3">
-        <v>80</v>
-      </c>
-      <c r="M212" s="3">
-        <v>84</v>
-      </c>
-      <c r="N212" s="3">
-        <v>87</v>
-      </c>
-      <c r="O212" s="3">
-        <v>90</v>
-      </c>
-      <c r="P212" s="3">
-        <v>94</v>
-      </c>
-      <c r="Q212" s="3">
-        <v>97</v>
-      </c>
-      <c r="R212" s="3">
-        <v>101</v>
-      </c>
-      <c r="S212" s="3">
-        <v>104</v>
-      </c>
-      <c r="T212" s="3">
-        <v>108</v>
-      </c>
-      <c r="U212" s="3">
-        <v>111</v>
-      </c>
-      <c r="V212" s="3">
-        <v>115</v>
-      </c>
-      <c r="W212" s="3">
-        <v>118</v>
-      </c>
-      <c r="X212" s="3">
-        <v>122</v>
-      </c>
-      <c r="Y212" s="3">
-        <v>125</v>
-      </c>
-      <c r="Z212" s="3">
-        <v>128</v>
-      </c>
-      <c r="AA212" s="3">
-        <v>132</v>
-      </c>
-      <c r="AB212" s="3">
-        <v>135</v>
-      </c>
-      <c r="AC212" s="3">
-        <v>139</v>
-      </c>
-      <c r="AD212" s="3">
-        <v>142</v>
-      </c>
-      <c r="AE212" s="3">
-        <v>146</v>
-      </c>
-      <c r="AF212" s="3">
-        <v>149</v>
-      </c>
-      <c r="AG212" s="3">
-        <v>153</v>
-      </c>
-      <c r="AH212" s="3">
-        <v>156</v>
-      </c>
-      <c r="AI212" s="3">
-        <v>159</v>
-      </c>
-      <c r="AJ212" s="3"/>
-      <c r="AK212" s="3"/>
-      <c r="AL212" s="3"/>
-      <c r="AM212" s="3"/>
-      <c r="AN212" s="3"/>
-      <c r="AO212" s="3"/>
-      <c r="AP212" s="3"/>
-      <c r="AQ212" s="3"/>
-      <c r="AR212" s="3"/>
-      <c r="AS212" s="3"/>
-      <c r="AT212" s="3"/>
-      <c r="AU212" s="3"/>
-      <c r="AV212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AW212" s="3"/>
-      <c r="AX212" s="3"/>
-      <c r="AY212" s="3"/>
-      <c r="AZ212" s="3"/>
-      <c r="BA212" s="3"/>
-      <c r="BB212" s="3"/>
-      <c r="BC212" s="3"/>
-      <c r="BD212" s="3"/>
-      <c r="BE212" s="3"/>
-      <c r="BF212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BG212" s="3"/>
-      <c r="BH212" s="3"/>
-      <c r="BI212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BJ212" s="3"/>
-      <c r="BK212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM212" s="3"/>
-      <c r="BN212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BP212" s="3"/>
-      <c r="BQ212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BR212" s="3"/>
-      <c r="BS212" s="3"/>
-      <c r="BT212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BU212" s="3"/>
-      <c r="BV212" s="3"/>
-      <c r="BW212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="BX212" s="3"/>
-      <c r="BY212" s="3"/>
-      <c r="BZ212" s="3"/>
-      <c r="CA212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="CB212" s="3"/>
-      <c r="CC212" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="CD212" s="3"/>
-      <c r="CE212" s="3"/>
-      <c r="CF212" s="1" t="str">
         <f t="shared" si="3"/>
         <v>YES</v>
       </c>

</xml_diff>